<commit_message>
Updated excel for datadriven
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EA204C4F-EDC7-449A-A713-6A45075D6C18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2DEE9C42-CA6A-4D3F-A34A-10889CAFF0A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Committing final changes for datadriver approach
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2DEE9C42-CA6A-4D3F-A34A-10889CAFF0A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{475A4A04-1483-473B-9B5C-759F56C34336}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated class files using test data reading from excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C55A8A3-2F0D-4FAB-800E-73D5E76C363B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C543BC20-D9AF-432C-A262-3FA1E5183419}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhoneBook" sheetId="1" r:id="rId1"/>
+    <sheet name="VendorSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Email</t>
   </si>
@@ -74,6 +75,33 @@
   </si>
   <si>
     <t>Internal Medicine (FIM)</t>
+  </si>
+  <si>
+    <t>JDEVendorSearch</t>
+  </si>
+  <si>
+    <t>VendorName</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>1618048</t>
+  </si>
+  <si>
+    <t>75266-0720</t>
   </si>
 </sst>
 </file>
@@ -143,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +189,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,4 +576,61 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D4407-1A58-41E2-99E7-738B49F4BC46}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test data, JDE vendor search login configured in XML file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C543BC20-D9AF-432C-A262-3FA1E5183419}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A2240E61-A027-4D62-99B5-3FCAD17FC288}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhoneBook" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Phone Book</t>
   </si>
   <si>
-    <t>Internal Medicine (FIM)</t>
-  </si>
-  <si>
     <t>JDEVendorSearch</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>75266-0720</t>
+  </si>
+  <si>
+    <t>Family Practice (FIM)</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D4407-1A58-41E2-99E7-738B49F4BC46}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -597,36 +597,36 @@
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored JDE Vendor search
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A2240E61-A027-4D62-99B5-3FCAD17FC288}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A20ABE3-DD30-433C-A7A3-DA99FE3B2B41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhoneBook" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>Family Practice (FIM)</t>
+  </si>
+  <si>
+    <t>HomePageTitle</t>
+  </si>
+  <si>
+    <t>Vendor Search Form</t>
+  </si>
+  <si>
+    <t>You have tried to access a secure area. Please enter your user name and password to gain access.</t>
+  </si>
+  <si>
+    <t>informationtex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not bookmark this page. Doing so will cause an error on your next visit. The correct procedure is to bookmark the page that appears after you click </t>
+  </si>
+  <si>
+    <t>alertTex</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>Not logged in</t>
   </si>
 </sst>
 </file>
@@ -482,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -580,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D4407-1A58-41E2-99E7-738B49F4BC46}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,16 +616,20 @@
     <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="5" width="19.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
@@ -614,8 +642,20 @@
       <c r="D2" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -627,6 +667,18 @@
       </c>
       <c r="D3" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tests to RejectedPractitioners
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A20ABE3-DD30-433C-A7A3-DA99FE3B2B41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A0D036F-1A87-497B-A63D-B2136CB619CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhoneBook" sheetId="1" r:id="rId1"/>
     <sheet name="VendorSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="GrossMarginEstimator" sheetId="4" r:id="rId3"/>
+    <sheet name="RejectedPractitioners" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>Email</t>
   </si>
@@ -74,6 +76,9 @@
     <t>Phone Book</t>
   </si>
   <si>
+    <t>Internal Medicine (FIM)</t>
+  </si>
+  <si>
     <t>JDEVendorSearch</t>
   </si>
   <si>
@@ -101,31 +106,223 @@
     <t>75266-0720</t>
   </si>
   <si>
-    <t>Family Practice (FIM)</t>
-  </si>
-  <si>
-    <t>HomePageTitle</t>
-  </si>
-  <si>
-    <t>Vendor Search Form</t>
-  </si>
-  <si>
-    <t>You have tried to access a secure area. Please enter your user name and password to gain access.</t>
-  </si>
-  <si>
-    <t>informationtex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not bookmark this page. Doing so will cause an error on your next visit. The correct procedure is to bookmark the page that appears after you click </t>
-  </si>
-  <si>
-    <t>alertTex</t>
-  </si>
-  <si>
-    <t>loginStatus</t>
-  </si>
-  <si>
-    <t>Not logged in</t>
+    <t>LoginGrossMarginEstimator</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>v_sthota</t>
+  </si>
+  <si>
+    <t>Hanuman@1</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>GrossMarginEstimatorElements</t>
+  </si>
+  <si>
+    <t>Worksite State:</t>
+  </si>
+  <si>
+    <t>Team:</t>
+  </si>
+  <si>
+    <t>Client Name:</t>
+  </si>
+  <si>
+    <t>Specialty:</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>Est # Practictioners:</t>
+  </si>
+  <si>
+    <t>#Hours/Shift:</t>
+  </si>
+  <si>
+    <t>#Work Day/Shifts:</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Contract Type</t>
+  </si>
+  <si>
+    <t>Inclusive</t>
+  </si>
+  <si>
+    <t>Per Diem</t>
+  </si>
+  <si>
+    <t>Bill Back</t>
+  </si>
+  <si>
+    <t>Rate:</t>
+  </si>
+  <si>
+    <t>OverTime:</t>
+  </si>
+  <si>
+    <t>OnCall Day:</t>
+  </si>
+  <si>
+    <t>OnCall Night:</t>
+  </si>
+  <si>
+    <t>#Hours/Day:</t>
+  </si>
+  <si>
+    <t>Rotation:</t>
+  </si>
+  <si>
+    <t>Job Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Info </t>
+  </si>
+  <si>
+    <t>LabelCount</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Get Default Days</t>
+  </si>
+  <si>
+    <t>Calculate</t>
+  </si>
+  <si>
+    <t>View Calendar</t>
+  </si>
+  <si>
+    <t>*Based on # of 8 hr. days: 0.0</t>
+  </si>
+  <si>
+    <t>Projected Gross Margin:</t>
+  </si>
+  <si>
+    <t>Client Rate:</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Malpractice/Day:</t>
+  </si>
+  <si>
+    <t>Air:</t>
+  </si>
+  <si>
+    <t>Rental Hsg/Day:</t>
+  </si>
+  <si>
+    <t>Rental Car/Day:</t>
+  </si>
+  <si>
+    <t>Licensing/Day:</t>
+  </si>
+  <si>
+    <t>Per Diems:</t>
+  </si>
+  <si>
+    <t>(Meals, Cars, Housing, etc)</t>
+  </si>
+  <si>
+    <t>Bonuses</t>
+  </si>
+  <si>
+    <t>Perks:</t>
+  </si>
+  <si>
+    <t>Mileage/Gas etc:</t>
+  </si>
+  <si>
+    <t>Other:</t>
+  </si>
+  <si>
+    <t>Based on Work Days</t>
+  </si>
+  <si>
+    <t>Benefits/Month:</t>
+  </si>
+  <si>
+    <t>Excise Tax/Day:</t>
+  </si>
+  <si>
+    <t>Bad Debt/Day:</t>
+  </si>
+  <si>
+    <t>Withholding/Day</t>
+  </si>
+  <si>
+    <t>Button Count</t>
+  </si>
+  <si>
+    <t>Work Unit:</t>
+  </si>
+  <si>
+    <t>Based on consecutive days (Car Days)</t>
+  </si>
+  <si>
+    <t>Work Days</t>
+  </si>
+  <si>
+    <t>RejectedPractitionersData</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>SocialSecurity</t>
+  </si>
+  <si>
+    <t>Johns</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>06/25/1975</t>
+  </si>
+  <si>
+    <t>565-79-5632</t>
   </si>
 </sst>
 </file>
@@ -195,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,6 +420,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,7 +708,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -604,10 +805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D4407-1A58-41E2-99E7-738B49F4BC46}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -616,73 +817,586 @@
     <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="10" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08BDED4-BE33-4259-88BA-D9C7124B2AED}">
+  <dimension ref="A1:D59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{83896F8F-A3BD-44C0-B543-AB88C8D8116B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB221B7-805C-48D6-A439-247261A892EC}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test data to excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A0D036F-1A87-497B-A63D-B2136CB619CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426C3092-ED57-4412-89F6-FB1023CBDF4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="3705" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
     <sheet name="VendorSearch" sheetId="2" r:id="rId2"/>
     <sheet name="GrossMarginEstimator" sheetId="4" r:id="rId3"/>
     <sheet name="RejectedPractitioners" sheetId="5" r:id="rId4"/>
+    <sheet name="QAEvals" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="167">
   <si>
     <t>Email</t>
   </si>
@@ -76,9 +77,6 @@
     <t>Phone Book</t>
   </si>
   <si>
-    <t>Internal Medicine (FIM)</t>
-  </si>
-  <si>
     <t>JDEVendorSearch</t>
   </si>
   <si>
@@ -115,12 +113,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>v_sthota</t>
-  </si>
-  <si>
-    <t>Hanuman@1</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -323,13 +315,223 @@
   </si>
   <si>
     <t>565-79-5632</t>
+  </si>
+  <si>
+    <t>ClassOfDisabledPagination</t>
+  </si>
+  <si>
+    <t>fg-button ui-button ui-state-default ui-state-disabled</t>
+  </si>
+  <si>
+    <t>Entry1</t>
+  </si>
+  <si>
+    <t>Entry2</t>
+  </si>
+  <si>
+    <t>Entry3</t>
+  </si>
+  <si>
+    <t>Entry4</t>
+  </si>
+  <si>
+    <t>Entry5</t>
+  </si>
+  <si>
+    <t>Entry6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Selected</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>HomePageTitle</t>
+  </si>
+  <si>
+    <t>Vendor Search Form</t>
+  </si>
+  <si>
+    <t>informationtex</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>alertText</t>
+  </si>
+  <si>
+    <t>You have tried to access a secure area. Please enter your user name and password to gain access.</t>
+  </si>
+  <si>
+    <t>Not logged in</t>
+  </si>
+  <si>
+    <t>Do not bookmark this page. Doing so will cause an error on your next visit. The correct procedure is to bookmark the page that appears after you click</t>
+  </si>
+  <si>
+    <t>QAEvalsTestData</t>
+  </si>
+  <si>
+    <t>clientEvalsPreTitle</t>
+  </si>
+  <si>
+    <t>providerEvalsTitle</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>assignmentEvalsTitle</t>
+  </si>
+  <si>
+    <t>QA Eval</t>
+  </si>
+  <si>
+    <t>clientEvalInAssignment</t>
+  </si>
+  <si>
+    <t>providerEvalInAssignment</t>
+  </si>
+  <si>
+    <t>editPageTitle</t>
+  </si>
+  <si>
+    <t>Report a technical problem</t>
+  </si>
+  <si>
+    <t>moreValue</t>
+  </si>
+  <si>
+    <t>View History</t>
+  </si>
+  <si>
+    <t>QA Evals</t>
+  </si>
+  <si>
+    <t>QAEvals</t>
+  </si>
+  <si>
+    <t>clientEvals</t>
+  </si>
+  <si>
+    <t>Client QA Evals</t>
+  </si>
+  <si>
+    <t>providerEvals</t>
+  </si>
+  <si>
+    <t>Client:</t>
+  </si>
+  <si>
+    <t>WorksiteState</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
+    <t>ClientName</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>MalPractice</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>OverTime</t>
+  </si>
+  <si>
+    <t>CallDay</t>
+  </si>
+  <si>
+    <t>CallNight</t>
+  </si>
+  <si>
+    <t>RatePayInfo</t>
+  </si>
+  <si>
+    <t>iseries</t>
+  </si>
+  <si>
+    <t>!$3r!3$T3$t</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>ALLER</t>
+  </si>
+  <si>
+    <t>CRW</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>11 Sep 2018</t>
+  </si>
+  <si>
+    <t>18 Sep 2018</t>
+  </si>
+  <si>
+    <t>75.08</t>
+  </si>
+  <si>
+    <t>50.08</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Provider QA Evals</t>
+  </si>
+  <si>
+    <t>FirstName_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Practice (FIM) </t>
+  </si>
+  <si>
+    <t>jon%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +560,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="30"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +592,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -392,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,10 +646,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -708,7 +953,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +1017,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D4407-1A58-41E2-99E7-738B49F4BC46}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -817,41 +1062,119 @@
     <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="5" width="25.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="10"/>
+    <col min="13" max="13" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="8" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
+      <c r="E3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -862,483 +1185,560 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08BDED4-BE33-4259-88BA-D9C7124B2AED}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="B9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B12" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B13" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B14" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>62</v>
+        <v>38</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>62</v>
+        <v>89</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>62</v>
+        <v>41</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>63</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>62</v>
+        <v>44</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>62</v>
+        <v>45</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>62</v>
+        <v>46</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>62</v>
+        <v>48</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>63</v>
+        <v>87</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>62</v>
+        <v>73</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>62</v>
+        <v>76</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>62</v>
+        <v>78</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>62</v>
+        <v>79</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>62</v>
+        <v>88</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>62</v>
+        <v>82</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>62</v>
+        <v>84</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>62</v>
+        <v>83</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>62</v>
+        <v>85</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{83896F8F-A3BD-44C0-B543-AB88C8D8116B}"/>
+    <hyperlink ref="B3" r:id="rId1" display="Hanuman@1" xr:uid="{BCB72F88-DFE8-4FD9-9A74-3C44093A8A6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1346,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB221B7-805C-48D6-A439-247261A892EC}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,17 +1758,18 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1376,27 +1777,130 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>99</v>
+      <c r="E4" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16858B1-939A-4726-9566-A92776824A1D}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="10"/>
+    <col min="9" max="9" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>